<commit_message>
Added Test-cases for ProductsAndServices Module.
</commit_message>
<xml_diff>
--- a/GUISeleniumFramework/testdata/testScriptdata.xlsx
+++ b/GUISeleniumFramework/testdata/testScriptdata.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHIDUSD\git\Dolibarr_GUIFramework_Testing\GUISeleniumFramework\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11625" windowHeight="6330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13005" windowHeight="4680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ThirdParty" sheetId="3" r:id="rId1"/>
-    <sheet name="productInvoice" sheetId="1" r:id="rId2"/>
-    <sheet name="UserGroups" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId4"/>
-    <sheet name="MRP" sheetId="5" r:id="rId5"/>
+    <sheet name="ProductsAndServices" sheetId="6" r:id="rId2"/>
+    <sheet name="productInvoice" sheetId="1" r:id="rId3"/>
+    <sheet name="UserGroups" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId5"/>
+    <sheet name="MRP" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="186">
   <si>
     <t>TC_ID</t>
   </si>
@@ -383,13 +389,211 @@
   </si>
   <si>
     <t>IREDA_</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>shortName</t>
+  </si>
+  <si>
+    <t>addIn</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>zipcode</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>fax</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>CreateInvoiceAndPaymentAndValidateForProspect</t>
+  </si>
+  <si>
+    <t>ClosingContractForProspect</t>
+  </si>
+  <si>
+    <t>CreateWarehouseAndProductAndVerify</t>
+  </si>
+  <si>
+    <t>CreateServicesAndVerifyInList</t>
+  </si>
+  <si>
+    <t>TC_09</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
+    <t>TC_12</t>
+  </si>
+  <si>
+    <t>Texas, USA.</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>United States (US)</t>
+  </si>
+  <si>
+    <t>RMW_001</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>75001</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>sellStatus</t>
+  </si>
+  <si>
+    <t>productRef</t>
+  </si>
+  <si>
+    <t>purchaseStatus</t>
+  </si>
+  <si>
+    <t>publicUrl</t>
+  </si>
+  <si>
+    <t>stockLimit</t>
+  </si>
+  <si>
+    <t>desiredStock</t>
+  </si>
+  <si>
+    <t>natureOfProduct</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> New_Warehouse_</t>
+  </si>
+  <si>
+    <t>NWH_</t>
+  </si>
+  <si>
+    <t>New_Warehouse_</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>customCode</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>sellingPrice</t>
+  </si>
+  <si>
+    <t>minSellingPrice</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>New_Prod_</t>
+  </si>
+  <si>
+    <t>For sale</t>
+  </si>
+  <si>
+    <t>For purchase</t>
+  </si>
+  <si>
+    <t>https://dolibarr/newprod_</t>
+  </si>
+  <si>
+    <t>Manufactured product</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>NPD_</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>2200</t>
+  </si>
+  <si>
+    <t>485</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>New_Service_</t>
+  </si>
+  <si>
+    <t>NSC_</t>
+  </si>
+  <si>
+    <t>https://dolibarr/newservice_</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>180</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -466,6 +670,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,7 +767,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -561,7 +802,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -738,21 +979,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
@@ -760,7 +1001,7 @@
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,7 +1018,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -792,14 +1033,14 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -816,7 +1057,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>108</v>
       </c>
@@ -831,14 +1072,14 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +1096,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -868,21 +1109,541 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="12" style="11" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="12" style="11" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" style="11" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="11"/>
+    <col min="14" max="14" width="13.7109375" style="11" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="11"/>
+    <col min="17" max="17" width="11.85546875" style="11" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" style="11" customWidth="1"/>
+    <col min="19" max="19" width="14" style="11" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" style="11" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+    </row>
+    <row r="2" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+    </row>
+    <row r="8" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="T9" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q10" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="S10" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="T10" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -890,7 +1651,7 @@
       <c r="E1" s="8"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -898,7 +1659,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -906,7 +1667,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -914,7 +1675,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -922,7 +1683,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -930,7 +1691,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -938,7 +1699,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -946,7 +1707,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -954,7 +1715,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -962,7 +1723,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -970,7 +1731,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -978,7 +1739,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -991,33 +1752,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
     </row>
@@ -1026,21 +1787,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1048,7 +1809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1056,7 +1817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1064,7 +1825,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1072,7 +1833,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1080,7 +1841,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1088,7 +1849,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1096,7 +1857,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1104,7 +1865,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1112,7 +1873,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1120,7 +1881,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1128,7 +1889,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1136,7 +1897,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1144,7 +1905,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1152,7 +1913,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1160,7 +1921,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -1168,7 +1929,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -1176,7 +1937,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -1184,7 +1945,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -1192,7 +1953,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -1200,7 +1961,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
@@ -1208,7 +1969,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
@@ -1216,7 +1977,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
@@ -1224,7 +1985,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
@@ -1232,7 +1993,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -1240,7 +2001,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -1248,7 +2009,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
@@ -1256,7 +2017,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -1264,7 +2025,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -1272,7 +2033,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>12</v>
       </c>
@@ -1280,7 +2041,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
@@ -1288,7 +2049,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>12</v>
       </c>
@@ -1296,7 +2057,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>12</v>
       </c>
@@ -1304,7 +2065,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>12</v>
       </c>
@@ -1312,7 +2073,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>12</v>
       </c>
@@ -1320,7 +2081,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>12</v>
       </c>
@@ -1328,7 +2089,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>12</v>
       </c>
@@ -1336,7 +2097,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>12</v>
       </c>
@@ -1344,7 +2105,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>12</v>
       </c>
@@ -1352,7 +2113,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>12</v>
       </c>
@@ -1360,7 +2121,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
@@ -1368,7 +2129,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>12</v>
       </c>
@@ -1376,7 +2137,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>12</v>
       </c>
@@ -1384,7 +2145,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>12</v>
       </c>
@@ -1392,7 +2153,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>12</v>
       </c>
@@ -1400,7 +2161,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>12</v>
       </c>
@@ -1408,7 +2169,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>12</v>
       </c>
@@ -1416,7 +2177,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>12</v>
       </c>
@@ -1424,7 +2185,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>12</v>
       </c>
@@ -1432,7 +2193,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>12</v>
       </c>
@@ -1440,7 +2201,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>56</v>
       </c>
@@ -1448,7 +2209,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>56</v>
       </c>
@@ -1456,7 +2217,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>56</v>
       </c>
@@ -1464,7 +2225,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>56</v>
       </c>
@@ -1472,7 +2233,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>56</v>
       </c>
@@ -1480,7 +2241,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>56</v>
       </c>
@@ -1488,7 +2249,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>56</v>
       </c>
@@ -1496,7 +2257,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>56</v>
       </c>
@@ -1504,7 +2265,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>56</v>
       </c>
@@ -1512,7 +2273,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>56</v>
       </c>
@@ -1520,7 +2281,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>56</v>
       </c>
@@ -1528,7 +2289,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>56</v>
       </c>
@@ -1536,7 +2297,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>56</v>
       </c>
@@ -1544,7 +2305,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>56</v>
       </c>
@@ -1552,7 +2313,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>56</v>
       </c>
@@ -1560,7 +2321,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>56</v>
       </c>
@@ -1568,7 +2329,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>56</v>
       </c>
@@ -1576,7 +2337,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>56</v>
       </c>
@@ -1584,7 +2345,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>56</v>
       </c>
@@ -1592,7 +2353,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>56</v>
       </c>
@@ -1600,7 +2361,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>56</v>
       </c>
@@ -1608,7 +2369,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>56</v>
       </c>
@@ -1616,7 +2377,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>56</v>
       </c>
@@ -1624,7 +2385,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>56</v>
       </c>
@@ -1632,7 +2393,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>56</v>
       </c>
@@ -1640,7 +2401,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>56</v>
       </c>
@@ -1648,7 +2409,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>56</v>
       </c>
@@ -1656,7 +2417,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>56</v>
       </c>
@@ -1664,7 +2425,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>56</v>
       </c>
@@ -1672,7 +2433,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>56</v>
       </c>
@@ -1680,7 +2441,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>56</v>
       </c>
@@ -1688,7 +2449,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>56</v>
       </c>
@@ -1696,7 +2457,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>56</v>
       </c>
@@ -1704,7 +2465,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>56</v>
       </c>
@@ -1712,7 +2473,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>56</v>
       </c>
@@ -1720,7 +2481,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>56</v>
       </c>
@@ -1728,7 +2489,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>56</v>
       </c>
@@ -1736,7 +2497,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>56</v>
       </c>
@@ -1744,7 +2505,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>56</v>
       </c>
@@ -1752,7 +2513,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>56</v>
       </c>
@@ -1760,7 +2521,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>56</v>
       </c>
@@ -1768,7 +2529,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>56</v>
       </c>
@@ -1776,7 +2537,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>56</v>
       </c>
@@ -1784,7 +2545,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>56</v>
       </c>
@@ -1792,7 +2553,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>56</v>
       </c>
@@ -1800,7 +2561,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>56</v>
       </c>
@@ -1808,7 +2569,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>56</v>
       </c>
@@ -1816,7 +2577,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>56</v>
       </c>
@@ -1824,7 +2585,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>56</v>
       </c>
@@ -1832,7 +2593,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>56</v>
       </c>
@@ -1845,15 +2606,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>